<commit_message>
Tile rotation and doors fixed
</commit_message>
<xml_diff>
--- a/Tiles.xlsx
+++ b/Tiles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitProjects\ZombieInMyPocket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157AEEC7-38C1-4260-AD0D-7B39A000B93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12AE683-D20F-4118-937D-2E80C98444B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29145" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{5021B4DD-1816-4D83-A9DE-5D0BD2A53050}"/>
+    <workbookView xWindow="-10725" yWindow="5430" windowWidth="21600" windowHeight="11385" xr2:uid="{5021B4DD-1816-4D83-A9DE-5D0BD2A53050}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -107,6 +107,18 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>North</t>
+  </si>
+  <si>
+    <t>East</t>
+  </si>
+  <si>
+    <t>South</t>
+  </si>
+  <si>
+    <t>West</t>
   </si>
 </sst>
 </file>
@@ -458,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30340054-06F0-475F-B068-0B6AA0F6ED56}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,7 +482,7 @@
     <col min="2" max="2" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -480,8 +492,20 @@
       <c r="C1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -491,8 +515,20 @@
       <c r="C2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -502,8 +538,20 @@
       <c r="C3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -513,8 +561,20 @@
       <c r="C4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -524,8 +584,20 @@
       <c r="C5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -535,8 +607,20 @@
       <c r="C6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -546,8 +630,20 @@
       <c r="C7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -557,8 +653,20 @@
       <c r="C8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -568,8 +676,20 @@
       <c r="C9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -579,8 +699,20 @@
       <c r="C10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -590,8 +722,20 @@
       <c r="C11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -601,8 +745,20 @@
       <c r="C12" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -612,8 +768,20 @@
       <c r="C13" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -623,8 +791,20 @@
       <c r="C14" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -634,8 +814,20 @@
       <c r="C15" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -645,8 +837,20 @@
       <c r="C16" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -655,6 +859,18 @@
       </c>
       <c r="C17" t="s">
         <v>20</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug Fixes and Output Improvements
Fixed a bug where moving back into the foyer after the first random tile was placed would invoke the Choosing door state as there was only one entrance.

Also Cleaned up some of the outputs
</commit_message>
<xml_diff>
--- a/Tiles.xlsx
+++ b/Tiles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitProjects\ZombieInMyPocket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12AE683-D20F-4118-937D-2E80C98444B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73BF0638-1755-41DC-B5FB-CA54118EC5A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10725" yWindow="5430" windowWidth="21600" windowHeight="11385" xr2:uid="{5021B4DD-1816-4D83-A9DE-5D0BD2A53050}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5021B4DD-1816-4D83-A9DE-5D0BD2A53050}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -473,13 +473,14 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>